<commit_message>
mejorando el requerimient 73
</commit_message>
<xml_diff>
--- a/Autorreporte/Requerimientos Reto Hackaton.xlsx
+++ b/Autorreporte/Requerimientos Reto Hackaton.xlsx
@@ -600,8 +600,8 @@
   </sheetPr>
   <dimension ref="A1:J144"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I65" activeCellId="0" sqref="I65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E68" activeCellId="0" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -681,7 +681,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="7" t="n">
         <f aca="false">SUM(J4:J103)</f>
-        <v>20</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3261,11 +3261,11 @@
         <v>3060</v>
       </c>
       <c r="I79" s="9" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
       <c r="J79" s="3" t="n">
         <f aca="false">IF(I79="Finalizado",H79,0)</f>
-        <v>0</v>
+        <v>3060</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
modificando segidor de requerimientos
</commit_message>
<xml_diff>
--- a/Autorreporte/Requerimientos Reto Hackaton.xlsx
+++ b/Autorreporte/Requerimientos Reto Hackaton.xlsx
@@ -600,8 +600,8 @@
   </sheetPr>
   <dimension ref="A1:J144"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E68" activeCellId="0" sqref="E68"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I69" activeCellId="0" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -681,7 +681,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="7" t="n">
         <f aca="false">SUM(J4:J103)</f>
-        <v>3080</v>
+        <v>3100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2887,11 +2887,11 @@
         <v>10</v>
       </c>
       <c r="I68" s="9" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
       <c r="J68" s="3" t="n">
         <f aca="false">IF(I68="Finalizado",H68,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2921,11 +2921,11 @@
         <v>10</v>
       </c>
       <c r="I69" s="9" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
       <c r="J69" s="3" t="n">
         <f aca="false">IF(I69="Finalizado",H69,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>